<commit_message>
Report & Design Archive Update
</commit_message>
<xml_diff>
--- a/Development/Design Archive/SIMON_stats.xlsx
+++ b/Development/Design Archive/SIMON_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis\Documents\Part III\3rd-Year-Project\Development\Design Archive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis\Documents\Part III\COMP3200\3rd-Year-Project\Development\Design Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01711BF1-1C47-4CA9-A829-4CDF786E7325}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBE07A4-C7A1-47B3-AC21-2B9958257068}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="7" xr2:uid="{EE9B88FB-1D0E-4AFA-A3BE-CC1D0DFF1109}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="2" xr2:uid="{EE9B88FB-1D0E-4AFA-A3BE-CC1D0DFF1109}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="89">
   <si>
     <t>Version</t>
   </si>
@@ -288,6 +288,18 @@
   <si>
     <t>Period</t>
   </si>
+  <si>
+    <t>426.36 mW</t>
+  </si>
+  <si>
+    <t>428.87 mW</t>
+  </si>
+  <si>
+    <t>428.88 mW</t>
+  </si>
+  <si>
+    <t>419.58 mW</t>
+  </si>
 </sst>
 </file>
 
@@ -1367,80 +1379,80 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6335,65 +6347,65 @@
       <selection activeCell="C3" sqref="C3:Z14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="9.1796875" style="1"/>
-    <col min="9" max="11" width="22.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="22.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="2.1796875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="8" width="9.140625" style="1"/>
+    <col min="9" max="11" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="2.1796875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.1796875" style="1"/>
+    <col min="23" max="23" width="2.140625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:26" ht="14.5" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="3:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C3" s="127" t="s">
+    <row r="2" spans="3:26" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="128"/>
-      <c r="E3" s="131" t="s">
+      <c r="D3" s="130"/>
+      <c r="E3" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="133"/>
-      <c r="I3" s="135" t="s">
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="137" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="136"/>
-      <c r="K3" s="136"/>
-      <c r="L3" s="136"/>
-      <c r="M3" s="136"/>
-      <c r="N3" s="136"/>
-      <c r="O3" s="136"/>
-      <c r="P3" s="137"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="138"/>
+      <c r="O3" s="138"/>
+      <c r="P3" s="139"/>
       <c r="Q3" s="38"/>
-      <c r="R3" s="131" t="s">
+      <c r="R3" s="133" t="s">
         <v>62</v>
       </c>
-      <c r="S3" s="132"/>
-      <c r="T3" s="132"/>
-      <c r="U3" s="132"/>
-      <c r="V3" s="133"/>
+      <c r="S3" s="134"/>
+      <c r="T3" s="134"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="135"/>
       <c r="W3" s="41"/>
-      <c r="X3" s="131" t="s">
+      <c r="X3" s="133" t="s">
         <v>64</v>
       </c>
-      <c r="Y3" s="132"/>
-      <c r="Z3" s="133"/>
+      <c r="Y3" s="134"/>
+      <c r="Z3" s="135"/>
     </row>
-    <row r="4" spans="3:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="129"/>
-      <c r="D4" s="130"/>
+    <row r="4" spans="3:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="131"/>
+      <c r="D4" s="132"/>
       <c r="E4" s="43" t="s">
         <v>8</v>
       </c>
@@ -6406,20 +6418,20 @@
       <c r="H4" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="127" t="s">
+      <c r="I4" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="134"/>
-      <c r="K4" s="134"/>
-      <c r="L4" s="128"/>
-      <c r="M4" s="127" t="s">
+      <c r="J4" s="136"/>
+      <c r="K4" s="136"/>
+      <c r="L4" s="130"/>
+      <c r="M4" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="128"/>
-      <c r="O4" s="127" t="s">
+      <c r="N4" s="130"/>
+      <c r="O4" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="128"/>
+      <c r="P4" s="130"/>
       <c r="Q4" s="39"/>
       <c r="R4" s="43" t="s">
         <v>68</v>
@@ -6447,7 +6459,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="3:26" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="27">
         <v>0</v>
       </c>
@@ -6518,7 +6530,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C6" s="11">
         <f t="shared" ref="C6:C13" si="0">C5+1</f>
         <v>1</v>
@@ -6588,7 +6600,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C7" s="11">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -6660,7 +6672,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C8" s="11">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6730,7 +6742,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C9" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6802,7 +6814,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C10" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6870,7 +6882,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C11" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6940,7 +6952,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="12" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C12" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7008,7 +7020,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="13" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C13" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7078,7 +7090,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="14" spans="3:26" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="3:26" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="18">
         <f t="shared" ref="C14" si="2">C13+1</f>
         <v>9</v>
@@ -7177,83 +7189,83 @@
       <selection activeCell="W5" sqref="W5:W15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="68"/>
-    <col min="3" max="3" width="1.90625" style="68" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.26953125" style="68" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.7109375" style="68"/>
+    <col min="3" max="3" width="1.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="68" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" style="68" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.54296875" style="68" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" style="68" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" style="68" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.90625" style="68" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.08984375" style="68" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.26953125" style="68" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.08984375" style="68" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" style="68" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" style="68" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="68" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" style="68" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="21.26953125" style="68" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.08984375" style="68" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="1.54296875" style="68" customWidth="1"/>
-    <col min="18" max="18" width="10.453125" style="68" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.453125" style="68" customWidth="1"/>
-    <col min="20" max="20" width="1.54296875" style="68" customWidth="1"/>
-    <col min="21" max="21" width="5.81640625" style="68" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.453125" style="68" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.6328125" style="68" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="1.54296875" style="68" customWidth="1"/>
-    <col min="25" max="25" width="5.81640625" style="99" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.08984375" style="99" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.453125" style="100" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.81640625" style="99" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.08984375" style="99" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.7265625" style="99" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.6328125" style="99" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="8.7265625" style="68"/>
+    <col min="13" max="15" width="21.28515625" style="68" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.140625" style="68" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.5703125" style="68" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" style="68" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" style="68" customWidth="1"/>
+    <col min="20" max="20" width="1.5703125" style="68" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" style="68" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.5703125" style="68" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="1.5703125" style="68" customWidth="1"/>
+    <col min="25" max="25" width="5.85546875" style="99" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.140625" style="99" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.42578125" style="100" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" style="99" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.140625" style="99" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.7109375" style="99" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" style="99" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="8.7109375" style="68"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:31" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="3:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="127" t="s">
+    <row r="3" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="128"/>
-      <c r="E4" s="131" t="s">
+      <c r="D4" s="130"/>
+      <c r="E4" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="139" t="s">
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
+      <c r="H4" s="135"/>
+      <c r="I4" s="141" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="140"/>
-      <c r="K4" s="140"/>
-      <c r="L4" s="140"/>
-      <c r="M4" s="140"/>
-      <c r="N4" s="140"/>
-      <c r="O4" s="140"/>
-      <c r="P4" s="140"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="142"/>
+      <c r="M4" s="142"/>
+      <c r="N4" s="142"/>
+      <c r="O4" s="142"/>
+      <c r="P4" s="142"/>
       <c r="Q4" s="47"/>
-      <c r="R4" s="146" t="s">
+      <c r="R4" s="148" t="s">
         <v>72</v>
       </c>
-      <c r="S4" s="147"/>
+      <c r="S4" s="149"/>
       <c r="T4" s="48"/>
-      <c r="U4" s="131" t="s">
+      <c r="U4" s="133" t="s">
         <v>64</v>
       </c>
-      <c r="V4" s="132"/>
-      <c r="W4" s="133"/>
+      <c r="V4" s="134"/>
+      <c r="W4" s="135"/>
       <c r="X4" s="106"/>
-      <c r="Y4" s="138"/>
-      <c r="Z4" s="138"/>
-      <c r="AA4" s="138"/>
-      <c r="AB4" s="138"/>
-      <c r="AC4" s="138"/>
-      <c r="AD4" s="138"/>
+      <c r="Y4" s="140"/>
+      <c r="Z4" s="140"/>
+      <c r="AA4" s="140"/>
+      <c r="AB4" s="140"/>
+      <c r="AC4" s="140"/>
+      <c r="AD4" s="140"/>
     </row>
-    <row r="5" spans="3:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="144"/>
-      <c r="D5" s="145"/>
+    <row r="5" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="146"/>
+      <c r="D5" s="147"/>
       <c r="E5" s="65" t="s">
         <v>8</v>
       </c>
@@ -7266,20 +7278,20 @@
       <c r="H5" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="139" t="s">
+      <c r="I5" s="141" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="140"/>
-      <c r="K5" s="140"/>
-      <c r="L5" s="141"/>
-      <c r="M5" s="142" t="s">
+      <c r="J5" s="142"/>
+      <c r="K5" s="142"/>
+      <c r="L5" s="143"/>
+      <c r="M5" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="143"/>
-      <c r="O5" s="142" t="s">
+      <c r="N5" s="145"/>
+      <c r="O5" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="143"/>
+      <c r="P5" s="145"/>
       <c r="Q5" s="51"/>
       <c r="R5" s="67" t="s">
         <v>73</v>
@@ -7305,7 +7317,7 @@
       <c r="AC5" s="101"/>
       <c r="AD5" s="102"/>
     </row>
-    <row r="6" spans="3:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C6" s="43">
         <v>0</v>
       </c>
@@ -7366,7 +7378,7 @@
       <c r="AD6" s="104"/>
       <c r="AE6" s="105"/>
     </row>
-    <row r="7" spans="3:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C7" s="25">
         <f t="shared" ref="C7:C15" si="0">C6+1</f>
         <v>1</v>
@@ -7426,7 +7438,7 @@
       <c r="AD7" s="104"/>
       <c r="AE7" s="105"/>
     </row>
-    <row r="8" spans="3:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C8" s="25">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -7488,7 +7500,7 @@
       <c r="AD8" s="104"/>
       <c r="AE8" s="105"/>
     </row>
-    <row r="9" spans="3:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C9" s="25">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -7548,7 +7560,7 @@
       <c r="AD9" s="104"/>
       <c r="AE9" s="105"/>
     </row>
-    <row r="10" spans="3:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C10" s="25">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7610,7 +7622,7 @@
       <c r="AD10" s="104"/>
       <c r="AE10" s="105"/>
     </row>
-    <row r="11" spans="3:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C11" s="25">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7668,7 +7680,7 @@
       <c r="AD11" s="104"/>
       <c r="AE11" s="105"/>
     </row>
-    <row r="12" spans="3:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C12" s="25">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7728,7 +7740,7 @@
       <c r="AD12" s="104"/>
       <c r="AE12" s="105"/>
     </row>
-    <row r="13" spans="3:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C13" s="25">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7786,7 +7798,7 @@
       <c r="AD13" s="104"/>
       <c r="AE13" s="105"/>
     </row>
-    <row r="14" spans="3:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C14" s="25">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7846,7 +7858,7 @@
       <c r="AD14" s="104"/>
       <c r="AE14" s="105"/>
     </row>
-    <row r="15" spans="3:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="26">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -7908,7 +7920,7 @@
       <c r="AD15" s="104"/>
       <c r="AE15" s="105"/>
     </row>
-    <row r="16" spans="3:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:31" x14ac:dyDescent="0.25">
       <c r="AD16" s="104"/>
     </row>
   </sheetData>
@@ -7930,111 +7942,113 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD09BB4-2C5C-435C-831B-8D251DCFFAEB}">
-  <dimension ref="C3:AM16"/>
+  <dimension ref="C3:AP16"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5:Y15"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AP7" sqref="AP7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="68"/>
-    <col min="3" max="3" width="1.90625" style="68" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.26953125" style="68" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.7109375" style="68"/>
+    <col min="3" max="3" width="1.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="68" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" style="68" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.54296875" style="68" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" style="68" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" style="68" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.90625" style="68" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.08984375" style="68" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.26953125" style="68" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.08984375" style="68" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" style="68" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" style="68" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="68" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" style="68" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.90625" style="68" customWidth="1"/>
-    <col min="14" max="16" width="21.26953125" style="68" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.08984375" style="68" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.08984375" style="68" customWidth="1"/>
-    <col min="19" max="19" width="1.54296875" style="68" customWidth="1"/>
-    <col min="20" max="20" width="10.453125" style="68" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.453125" style="68" customWidth="1"/>
-    <col min="22" max="22" width="1.54296875" style="68" customWidth="1"/>
-    <col min="23" max="23" width="5.81640625" style="68" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.453125" style="68" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.6328125" style="68" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="1.54296875" style="68" customWidth="1"/>
-    <col min="27" max="27" width="5.81640625" style="68" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" style="68" customWidth="1"/>
+    <col min="14" max="16" width="21.28515625" style="68" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" style="68" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" style="68" customWidth="1"/>
+    <col min="19" max="19" width="1.5703125" style="68" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" style="68" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" style="68" customWidth="1"/>
+    <col min="22" max="22" width="1.5703125" style="68" customWidth="1"/>
+    <col min="23" max="23" width="5.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.42578125" style="68" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5703125" style="68" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="1.5703125" style="68" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" style="68" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="68" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.81640625" style="68" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.453125" style="69" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.453125" style="69" customWidth="1"/>
-    <col min="32" max="32" width="8.81640625" style="68" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="8.81640625" style="68" customWidth="1"/>
+    <col min="29" max="29" width="6.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.42578125" style="69" customWidth="1"/>
+    <col min="32" max="32" width="8.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="8.85546875" style="68" customWidth="1"/>
     <col min="35" max="35" width="8" style="68" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.81640625" style="68" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.7265625" style="68" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.7265625" style="68" customWidth="1"/>
-    <col min="39" max="39" width="10.6328125" style="68" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="8.7265625" style="68"/>
+    <col min="36" max="36" width="6.85546875" style="68" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.7109375" style="68" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.7109375" style="68" customWidth="1"/>
+    <col min="39" max="39" width="10.5703125" style="68" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.7109375" style="68"/>
+    <col min="41" max="42" width="10.5703125" style="68" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="8.7109375" style="68"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:39" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="3:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="127" t="s">
+    <row r="3" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="128"/>
-      <c r="E4" s="131" t="s">
+      <c r="D4" s="130"/>
+      <c r="E4" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="139" t="s">
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
+      <c r="H4" s="135"/>
+      <c r="I4" s="141" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="140"/>
-      <c r="K4" s="140"/>
-      <c r="L4" s="140"/>
-      <c r="M4" s="140"/>
-      <c r="N4" s="140"/>
-      <c r="O4" s="140"/>
-      <c r="P4" s="140"/>
-      <c r="Q4" s="140"/>
-      <c r="R4" s="141"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="142"/>
+      <c r="M4" s="142"/>
+      <c r="N4" s="142"/>
+      <c r="O4" s="142"/>
+      <c r="P4" s="142"/>
+      <c r="Q4" s="142"/>
+      <c r="R4" s="143"/>
       <c r="S4" s="47"/>
-      <c r="T4" s="146" t="s">
+      <c r="T4" s="148" t="s">
         <v>72</v>
       </c>
-      <c r="U4" s="147"/>
+      <c r="U4" s="149"/>
       <c r="V4" s="48"/>
-      <c r="W4" s="131" t="s">
+      <c r="W4" s="133" t="s">
         <v>64</v>
       </c>
-      <c r="X4" s="132"/>
-      <c r="Y4" s="133"/>
+      <c r="X4" s="134"/>
+      <c r="Y4" s="135"/>
       <c r="Z4" s="110"/>
-      <c r="AA4" s="148" t="s">
+      <c r="AA4" s="150" t="s">
         <v>76</v>
       </c>
-      <c r="AB4" s="149"/>
-      <c r="AC4" s="149"/>
-      <c r="AD4" s="149"/>
-      <c r="AE4" s="150"/>
-      <c r="AF4" s="148" t="s">
+      <c r="AB4" s="151"/>
+      <c r="AC4" s="151"/>
+      <c r="AD4" s="151"/>
+      <c r="AE4" s="152"/>
+      <c r="AF4" s="150" t="s">
         <v>78</v>
       </c>
-      <c r="AG4" s="149"/>
-      <c r="AH4" s="149"/>
-      <c r="AI4" s="149"/>
-      <c r="AJ4" s="149"/>
-      <c r="AK4" s="149"/>
-      <c r="AL4" s="150"/>
+      <c r="AG4" s="151"/>
+      <c r="AH4" s="151"/>
+      <c r="AI4" s="151"/>
+      <c r="AJ4" s="151"/>
+      <c r="AK4" s="151"/>
+      <c r="AL4" s="152"/>
       <c r="AM4" s="92" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="3:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="144"/>
-      <c r="D5" s="145"/>
+    <row r="5" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="146"/>
+      <c r="D5" s="147"/>
       <c r="E5" s="58" t="s">
         <v>8</v>
       </c>
@@ -8047,23 +8061,23 @@
       <c r="H5" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="139" t="s">
+      <c r="I5" s="141" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="140"/>
-      <c r="K5" s="140"/>
-      <c r="L5" s="141"/>
+      <c r="J5" s="142"/>
+      <c r="K5" s="142"/>
+      <c r="L5" s="143"/>
       <c r="M5" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="142" t="s">
+      <c r="N5" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="143"/>
-      <c r="P5" s="142" t="s">
+      <c r="O5" s="145"/>
+      <c r="P5" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="143"/>
+      <c r="Q5" s="145"/>
       <c r="R5" s="64" t="s">
         <v>80</v>
       </c>
@@ -8121,7 +8135,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="3:39" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C6" s="43">
         <v>0</v>
       </c>
@@ -8227,8 +8241,14 @@
         <f>AK6/AD6</f>
         <v>3.0294806334139093</v>
       </c>
+      <c r="AO6" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="AP6" s="68" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="7" spans="3:39" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C7" s="11">
         <f t="shared" ref="C7:C14" si="0">C6+1</f>
         <v>1</v>
@@ -8334,8 +8354,14 @@
         <f t="shared" ref="AM7:AM15" si="8">AK7/AD7</f>
         <v>2.5327783734497289</v>
       </c>
+      <c r="AO7" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP7" s="68" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="8" spans="3:39" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C8" s="11">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -8443,8 +8469,11 @@
         <f t="shared" si="8"/>
         <v>2.5327783734497289</v>
       </c>
+      <c r="AO8" s="68" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="9" spans="3:39" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C9" s="11">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -8551,7 +8580,7 @@
         <v>3.0991835588312209</v>
       </c>
     </row>
-    <row r="10" spans="3:39" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C10" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8660,7 +8689,7 @@
         <v>3.2928825312581727</v>
       </c>
     </row>
-    <row r="11" spans="3:39" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C11" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8765,7 +8794,7 @@
         <v>3.7707834981087163</v>
       </c>
     </row>
-    <row r="12" spans="3:39" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C12" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8872,7 +8901,7 @@
         <v>4.0064574667405113</v>
       </c>
     </row>
-    <row r="13" spans="3:39" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C13" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -8977,7 +9006,7 @@
         <v>3.6197347940974192</v>
       </c>
     </row>
-    <row r="14" spans="3:39" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C14" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -9084,7 +9113,7 @@
         <v>3.6197347940974192</v>
       </c>
     </row>
-    <row r="15" spans="3:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="18">
         <f t="shared" ref="C15" si="10">C14+1</f>
         <v>9</v>
@@ -9193,7 +9222,7 @@
         <v>3.8610504470372473</v>
       </c>
     </row>
-    <row r="16" spans="3:39" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:42" x14ac:dyDescent="0.25">
       <c r="AK16" s="70"/>
       <c r="AL16" s="70"/>
       <c r="AM16" s="68">
@@ -9225,13 +9254,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9921E2F8-A528-4B54-889B-D2639774D815}">
   <dimension ref="C3:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="97" t="s">
         <v>65</v>
       </c>
@@ -9251,7 +9280,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="43">
         <v>437</v>
       </c>
@@ -9262,7 +9291,7 @@
         <f>D4-C4</f>
         <v>198</v>
       </c>
-      <c r="F4" s="151">
+      <c r="F4" s="127">
         <f>E4/C4</f>
         <v>0.45308924485125857</v>
       </c>
@@ -9276,7 +9305,7 @@
         <f>I4-H4</f>
         <v>373</v>
       </c>
-      <c r="K4" s="151">
+      <c r="K4" s="127">
         <f>J4/H4</f>
         <v>0.56859756097560976</v>
       </c>
@@ -9290,12 +9319,12 @@
         <f>N4-M4</f>
         <v>29</v>
       </c>
-      <c r="P4" s="151">
+      <c r="P4" s="127">
         <f>O4/M4</f>
         <v>0.21014492753623187</v>
       </c>
     </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="93">
         <v>717</v>
       </c>
@@ -9306,7 +9335,7 @@
         <f t="shared" ref="E5:E13" si="0">D5-C5</f>
         <v>254</v>
       </c>
-      <c r="F5" s="151">
+      <c r="F5" s="127">
         <f t="shared" ref="F5:F13" si="1">E5/C5</f>
         <v>0.35425383542538352</v>
       </c>
@@ -9320,7 +9349,7 @@
         <f t="shared" ref="J5:J13" si="2">I5-H5</f>
         <v>493</v>
       </c>
-      <c r="K5" s="151">
+      <c r="K5" s="127">
         <f t="shared" ref="K5:K13" si="3">J5/H5</f>
         <v>0.46997140133460441</v>
       </c>
@@ -9334,12 +9363,12 @@
         <f t="shared" ref="O5:O13" si="4">N5-M5</f>
         <v>53</v>
       </c>
-      <c r="P5" s="151">
+      <c r="P5" s="127">
         <f t="shared" ref="P5:P13" si="5">O5/M5</f>
         <v>0.29775280898876405</v>
       </c>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" s="93">
         <v>730</v>
       </c>
@@ -9350,7 +9379,7 @@
         <f t="shared" si="0"/>
         <v>267</v>
       </c>
-      <c r="F6" s="151">
+      <c r="F6" s="127">
         <f t="shared" si="1"/>
         <v>0.36575342465753424</v>
       </c>
@@ -9364,7 +9393,7 @@
         <f t="shared" si="2"/>
         <v>517</v>
       </c>
-      <c r="K6" s="151">
+      <c r="K6" s="127">
         <f t="shared" si="3"/>
         <v>0.48182665424044735</v>
       </c>
@@ -9378,12 +9407,12 @@
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="P6" s="151">
+      <c r="P6" s="127">
         <f t="shared" si="5"/>
         <v>0.14356435643564355</v>
       </c>
     </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" s="93">
         <v>1123</v>
       </c>
@@ -9394,7 +9423,7 @@
         <f t="shared" si="0"/>
         <v>323</v>
       </c>
-      <c r="F7" s="151">
+      <c r="F7" s="127">
         <f t="shared" si="1"/>
         <v>0.28762243989314334</v>
       </c>
@@ -9408,7 +9437,7 @@
         <f t="shared" si="2"/>
         <v>629</v>
       </c>
-      <c r="K7" s="151">
+      <c r="K7" s="127">
         <f t="shared" si="3"/>
         <v>0.39684542586750787</v>
       </c>
@@ -9422,12 +9451,12 @@
         <f t="shared" si="4"/>
         <v>61</v>
       </c>
-      <c r="P7" s="151">
+      <c r="P7" s="127">
         <f t="shared" si="5"/>
         <v>0.2606837606837607</v>
       </c>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" s="93">
         <v>1123</v>
       </c>
@@ -9438,7 +9467,7 @@
         <f t="shared" si="0"/>
         <v>334</v>
       </c>
-      <c r="F8" s="151">
+      <c r="F8" s="127">
         <f t="shared" si="1"/>
         <v>0.29741763134461263</v>
       </c>
@@ -9452,7 +9481,7 @@
         <f t="shared" si="2"/>
         <v>661</v>
       </c>
-      <c r="K8" s="151">
+      <c r="K8" s="127">
         <f t="shared" si="3"/>
         <v>0.39321832242712673</v>
       </c>
@@ -9466,12 +9495,12 @@
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="P8" s="151">
+      <c r="P8" s="127">
         <f t="shared" si="5"/>
         <v>0.10902255639097744</v>
       </c>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9" s="93">
         <v>1905</v>
       </c>
@@ -9482,7 +9511,7 @@
         <f t="shared" si="0"/>
         <v>432</v>
       </c>
-      <c r="F9" s="151">
+      <c r="F9" s="127">
         <f t="shared" si="1"/>
         <v>0.22677165354330708</v>
       </c>
@@ -9496,7 +9525,7 @@
         <f t="shared" si="2"/>
         <v>853</v>
       </c>
-      <c r="K9" s="151">
+      <c r="K9" s="127">
         <f t="shared" si="3"/>
         <v>0.30453409496608352</v>
       </c>
@@ -9510,12 +9539,12 @@
         <f t="shared" si="4"/>
         <v>125</v>
       </c>
-      <c r="P9" s="151">
+      <c r="P9" s="127">
         <f t="shared" si="5"/>
         <v>0.41946308724832215</v>
       </c>
     </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" s="93">
         <v>2024</v>
       </c>
@@ -9526,7 +9555,7 @@
         <f t="shared" si="0"/>
         <v>477</v>
       </c>
-      <c r="F10" s="151">
+      <c r="F10" s="127">
         <f t="shared" si="1"/>
         <v>0.23567193675889328</v>
       </c>
@@ -9540,7 +9569,7 @@
         <f t="shared" si="2"/>
         <v>901</v>
       </c>
-      <c r="K10" s="151">
+      <c r="K10" s="127">
         <f t="shared" si="3"/>
         <v>0.30594227504244481</v>
       </c>
@@ -9554,12 +9583,12 @@
         <f t="shared" si="4"/>
         <v>77</v>
       </c>
-      <c r="P10" s="151">
+      <c r="P10" s="127">
         <f t="shared" si="5"/>
         <v>0.22254335260115607</v>
       </c>
     </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" s="93">
         <v>3266</v>
       </c>
@@ -9570,7 +9599,7 @@
         <f t="shared" si="0"/>
         <v>547</v>
       </c>
-      <c r="F11" s="151">
+      <c r="F11" s="127">
         <f t="shared" si="1"/>
         <v>0.16748315982853643</v>
       </c>
@@ -9584,7 +9613,7 @@
         <f t="shared" si="2"/>
         <v>1109</v>
       </c>
-      <c r="K11" s="151">
+      <c r="K11" s="127">
         <f t="shared" si="3"/>
         <v>0.23327724021876314</v>
       </c>
@@ -9598,12 +9627,12 @@
         <f t="shared" si="4"/>
         <v>157</v>
       </c>
-      <c r="P11" s="151">
+      <c r="P11" s="127">
         <f t="shared" si="5"/>
         <v>0.39847715736040606</v>
       </c>
     </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="93">
         <v>3627</v>
       </c>
@@ -9614,7 +9643,7 @@
         <f t="shared" si="0"/>
         <v>488</v>
       </c>
-      <c r="F12" s="151">
+      <c r="F12" s="127">
         <f t="shared" si="1"/>
         <v>0.13454645712710228</v>
       </c>
@@ -9628,7 +9657,7 @@
         <f t="shared" si="2"/>
         <v>1173</v>
       </c>
-      <c r="K12" s="151">
+      <c r="K12" s="127">
         <f t="shared" si="3"/>
         <v>0.24027038099139697</v>
       </c>
@@ -9642,12 +9671,12 @@
         <f t="shared" si="4"/>
         <v>93</v>
       </c>
-      <c r="P12" s="151">
+      <c r="P12" s="127">
         <f t="shared" si="5"/>
         <v>0.20305676855895197</v>
       </c>
     </row>
-    <row r="13" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="95">
         <v>3498</v>
       </c>
@@ -9658,7 +9687,7 @@
         <f t="shared" si="0"/>
         <v>619</v>
       </c>
-      <c r="F13" s="151">
+      <c r="F13" s="127">
         <f t="shared" si="1"/>
         <v>0.17695826186392224</v>
       </c>
@@ -9672,7 +9701,7 @@
         <f t="shared" si="2"/>
         <v>1237</v>
       </c>
-      <c r="K13" s="151">
+      <c r="K13" s="127">
         <f t="shared" si="3"/>
         <v>0.24075515764889061</v>
       </c>
@@ -9686,20 +9715,20 @@
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="P13" s="151">
+      <c r="P13" s="127">
         <f t="shared" si="5"/>
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="K14" s="151"/>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="K14" s="127"/>
     </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="E15" s="152">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E15" s="128">
         <f>AVERAGE(E4:E13)</f>
         <v>393.9</v>
       </c>
-      <c r="F15" s="151">
+      <c r="F15" s="127">
         <f>AVERAGE(F4:F13)</f>
         <v>0.26995680452936932</v>
       </c>
@@ -9707,7 +9736,7 @@
         <f>AVERAGE(J4:J13)</f>
         <v>794.6</v>
       </c>
-      <c r="K15" s="151">
+      <c r="K15" s="127">
         <f>AVERAGE(K4:K13)</f>
         <v>0.36352385137128745</v>
       </c>
@@ -9715,7 +9744,7 @@
         <f>AVERAGE(O4:O13)</f>
         <v>68.2</v>
       </c>
-      <c r="P15" s="151">
+      <c r="P15" s="127">
         <f>AVERAGE(P4:P13)</f>
         <v>0.23202643313597693</v>
       </c>

</xml_diff>